<commit_message>
basic listing of Goals
</commit_message>
<xml_diff>
--- a/Teams/Goals.xlsx
+++ b/Teams/Goals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryannleslie/Documents/Study/cse210/Teams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F72F19-2F8C-304D-A88F-7F826037DF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E5EEBC-DE77-AF4D-84D1-5D1FE1AFF80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1120" windowWidth="26920" windowHeight="16940" xr2:uid="{FC2AE6C8-62E2-9A44-A9A5-EF4B7A526443}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Menu</t>
   </si>
@@ -128,13 +128,37 @@
   </si>
   <si>
     <t>_IsComplete: bool</t>
+  </si>
+  <si>
+    <t>create a goal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu </t>
+  </si>
+  <si>
+    <t>List goals</t>
+  </si>
+  <si>
+    <t>GoaltoList(): List&lt;Goals&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DisplayMenu() ---&gt; DisplayGoalTypes ---&gt; Create the Goal ---&gt; GoalToList()</t>
+  </si>
+  <si>
+    <t>_goalList: List&lt;Goals&gt;</t>
+  </si>
+  <si>
+    <t>DisplayGoals(): void</t>
+  </si>
+  <si>
+    <t>DisplayMenu() ---&gt; DisplayGoals()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,6 +177,61 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,16 +304,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5BDCE5D-40D2-BF4C-B341-5B5B5F054B8B}">
-  <dimension ref="B1:L20"/>
+  <dimension ref="B1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -571,24 +667,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -639,7 +735,9 @@
       <c r="B6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="J6" s="4"/>
       <c r="L6" s="4"/>
@@ -677,87 +775,133 @@
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="4"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D12" s="5" t="s">
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="6"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F14" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D13" s="3" t="s">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D14" s="3" t="s">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="3" t="s">
+      <c r="F17" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="3" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>